<commit_message>
Beta 0.9.3 - Fixed files
</commit_message>
<xml_diff>
--- a/config/NTDS_Template_captains.xlsx
+++ b/config/NTDS_Template_captains.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alen\PycharmProjects\NTDS_Loting\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alen\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="17400" windowWidth="28800" windowHeight="12195"/>
+    <workbookView xWindow="0" yWindow="18000" windowWidth="28800" windowHeight="12195"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
   <si>
     <t>E-mail</t>
   </si>
@@ -127,6 +127,9 @@
   </si>
   <si>
     <t>Tussen-voegsel</t>
+  </si>
+  <si>
+    <t>Nee</t>
   </si>
 </sst>
 </file>
@@ -491,7 +494,7 @@
   <dimension ref="A1:X201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="W2" sqref="W2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -6188,7 +6191,7 @@
       <c r="W201" s="3"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="oOEdjcOgQjWMU1v6hlcXJWw0WXWAD2HJLIfO1oB104zKuDUT4pWLJgJiJy74aMRF8ThJr6DDPcXtl+ZKTgouQQ==" saltValue="E1hBS8JTXLi9E0UPFsoMPg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="glg3FtY7gBqEuH7u0V2twGAvztHer/NaNr0O1gnPpukYYFrKagZ9L5LI8BiwoEeKQzJpHFJMlcDnGy+sjxQ1Dw==" saltValue="woMZkdiZ/r3RvlMrY0H/0A==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <dataValidations count="2">
     <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:I201">
       <formula1>0</formula1>
@@ -6199,7 +6202,7 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>AllowedValues!$B$3:$B$4</xm:f>
@@ -6208,21 +6211,33 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>AllowedValues!$C$3</xm:f>
+            <xm:f>AllowedValues!$C$3:$C$4</xm:f>
           </x14:formula1>
-          <xm:sqref>S2:T201 W2:W201 L2:N201</xm:sqref>
+          <xm:sqref>W2:W201</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>AllowedValues!$D$3:$D$4</xm:f>
+            <xm:f>AllowedValues!$D$3:$D$5</xm:f>
           </x14:formula1>
-          <xm:sqref>V2:V201 O2:R201</xm:sqref>
+          <xm:sqref>V2:V201</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>AllowedValues!$A$3:$A$5</xm:f>
           </x14:formula1>
           <xm:sqref>F2:G201</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>AllowedValues!$C$3:$C$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>L2:N201 S2:T201</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>AllowedValues!$D$3:$D$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>O2:R201</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -6235,7 +6250,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6275,6 +6290,9 @@
       <c r="B4" t="s">
         <v>26</v>
       </c>
+      <c r="C4" t="s">
+        <v>34</v>
+      </c>
       <c r="D4" t="s">
         <v>32</v>
       </c>
@@ -6283,9 +6301,12 @@
       <c r="A5" t="s">
         <v>24</v>
       </c>
+      <c r="D5" t="s">
+        <v>34</v>
+      </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="iHyqE66AwEg+zz/SQGMdEYKVWuMJFHEg2sIGEyOd6OHUDhgYB/nXOrAr1VQsWgwkIjrAZu0aLmz/Thn9/NQiag==" saltValue="pz7a22TuJVhgg8ycTq+hZg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="oLr/HvhKzAvLWmqolyqchiRHBXdVvafj4HyrhNvPEyCS+nocb5JO6hBmesEFPa18R+aiqpGm3I9iAATBALIEEg==" saltValue="1Gg3QnFA+18OmSjhwCknNQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>